<commit_message>
Update Chapter 7 - Beyond the Basic LAN.xlsx
</commit_message>
<xml_diff>
--- a/Chapter 7 - Beyond the Basic LAN.xlsx
+++ b/Chapter 7 - Beyond the Basic LAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CompTIA\Security+\SY0-501\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E119E2-FB4B-4287-A893-2E9C566DED54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A51A81-7F88-4194-A3B2-7D5A636B8758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -261,7 +261,79 @@
     <t>Type 2 Hypervisor</t>
   </si>
   <si>
-    <t>Runs inside of an operating system of a physical host machine</t>
+    <t>Virtual Security</t>
+  </si>
+  <si>
+    <t>Runs inside of an operating system of a physical host machine. E.g. VirtualBox</t>
+  </si>
+  <si>
+    <t>Security features, patch management, hardware maintenance, resilient and high availability</t>
+  </si>
+  <si>
+    <t>Virtualization characteristics</t>
+  </si>
+  <si>
+    <t>Network Separation</t>
+  </si>
+  <si>
+    <t>Snapshots and backups</t>
+  </si>
+  <si>
+    <t>Separate VMs on one server using virtual switch</t>
+  </si>
+  <si>
+    <t>Easy to backup, save states, debug</t>
+  </si>
+  <si>
+    <t>Virtual Threats</t>
+  </si>
+  <si>
+    <t>Anything that can happen to VM can happen to physical machine</t>
+  </si>
+  <si>
+    <t>VM Sprawl</t>
+  </si>
+  <si>
+    <t>Various virtual machines with no centralization - bad thing</t>
+  </si>
+  <si>
+    <t>VM Escape</t>
+  </si>
+  <si>
+    <t>Escapes VM and affects host system</t>
+  </si>
+  <si>
+    <t>Hardening Virtualization</t>
+  </si>
+  <si>
+    <t>Remove remnant data, make good policies, define user privileges, patch everything</t>
+  </si>
+  <si>
+    <t>Cloud Acess Security Broker</t>
+  </si>
+  <si>
+    <t>Intermediary between local infrastructure and the cloud. Usually on the cloud. Watches for malware, and controls policies</t>
+  </si>
+  <si>
+    <t>Containerisation</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Runs isolated instances of programs and services</t>
+  </si>
+  <si>
+    <t>Self-contained application that communicates with network resources that are permitted</t>
+  </si>
+  <si>
+    <t>Containers can depend on each other and can be configured to communicate on a single host</t>
+  </si>
+  <si>
+    <t>&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Containers run a single program with all its dependencies until it's closed</t>
   </si>
 </sst>
 </file>
@@ -579,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +973,109 @@
         <v>77</v>
       </c>
       <c r="C36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>